<commit_message>
AutoCommit_26 июня 2024 г. 12:19:44_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_ТерВер.xlsx
+++ b/2ИСИП-222_ТерВер.xlsx
@@ -563,10 +563,10 @@
   <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U40" sqref="T40:U40"/>
+      <selection pane="bottomRight" activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>